<commit_message>
All feedback changes done
</commit_message>
<xml_diff>
--- a/TestData/editVCenterData.xlsx
+++ b/TestData/editVCenterData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEC58A8-6E04-47A7-B99D-061FEB3AFAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C959DEB2-665B-44B5-8016-C40F208E2E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1932" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>